<commit_message>
adding filtering model, adding first mvp of a user interface and api
</commit_message>
<xml_diff>
--- a/collaborative_filtering/updated_dataset.xlsx
+++ b/collaborative_filtering/updated_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG211"/>
+  <dimension ref="A1:AH211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,6 +599,11 @@
           <t>metric_18</t>
         </is>
       </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>agile_methods_split</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -631,7 +636,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -680,6 +685,11 @@
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -712,7 +722,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -777,6 +787,11 @@
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -809,7 +824,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -870,6 +885,11 @@
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -902,7 +922,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -963,6 +983,11 @@
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
       <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -995,7 +1020,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1052,6 +1077,11 @@
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1084,7 +1114,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean, Safe</t>
+          <t>['Scrum', 'Kanban', 'Lean', 'Safe']</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -1149,6 +1179,11 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean', 'Safe']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1181,7 +1216,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1246,6 +1281,11 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr"/>
       <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1278,7 +1318,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Kanban</t>
+          <t>['Kanban']</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1339,6 +1379,11 @@
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr"/>
       <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>['Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1371,7 +1416,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1428,6 +1473,11 @@
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr"/>
       <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1460,7 +1510,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1488,7 +1538,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Throughput, Clima</t>
+          <t>Throughput</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1525,6 +1575,11 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr"/>
       <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1557,7 +1612,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Scrum, Lean</t>
+          <t>['Scrum', 'Lean']</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1593,7 +1648,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Lead time, Delivery to customer, Roadmaps</t>
+          <t>Lead time, Roadmaps</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1634,6 +1689,11 @@
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="inlineStr"/>
       <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1666,7 +1726,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -1731,6 +1791,11 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="inlineStr"/>
       <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1763,7 +1828,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1840,6 +1905,11 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="inlineStr"/>
       <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1872,7 +1942,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -1925,6 +1995,11 @@
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" t="inlineStr"/>
       <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1957,7 +2032,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -2022,6 +2097,11 @@
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr"/>
       <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2054,7 +2134,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -2119,6 +2199,11 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="inlineStr"/>
       <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2151,7 +2236,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -2224,6 +2309,11 @@
       <c r="AE18" t="inlineStr"/>
       <c r="AF18" t="inlineStr"/>
       <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2256,7 +2346,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -2309,6 +2399,11 @@
       <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr"/>
       <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2341,7 +2436,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -2402,6 +2497,11 @@
       <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="inlineStr"/>
       <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2434,7 +2534,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Scrum, Safe</t>
+          <t>['Scrum', 'Safe']</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -2499,6 +2599,11 @@
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr"/>
       <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Safe']</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2531,7 +2636,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -2555,7 +2660,7 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Throughput, Cycle time, Lead time, CFD, Cumulative Flow Diagrams, Number of completed tasks, Roadmaps, Velocity, Throughput, NPS</t>
+          <t>Throughput, Cycle time, Lead time, CFD, Number of completed tasks, Roadmaps, Velocity, Throughput, NPS</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2620,6 +2725,11 @@
       <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="inlineStr"/>
       <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2652,7 +2762,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>kanban adaptado baseado em drive domain design</t>
+          <t>['Kanban']</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2688,7 +2798,7 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Roadmaps, Velocity, Cumulative Flow Diagrams, Clima, Number of remaining tasks</t>
+          <t>Roadmaps, Velocity, Number of remaining tasks</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2733,6 +2843,11 @@
       <c r="AE23" t="inlineStr"/>
       <c r="AF23" t="inlineStr"/>
       <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr">
+        <is>
+          <t>['Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2765,7 +2880,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
@@ -2822,6 +2937,11 @@
       <c r="AE24" t="inlineStr"/>
       <c r="AF24" t="inlineStr"/>
       <c r="AG24" t="inlineStr"/>
+      <c r="AH24" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2854,7 +2974,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2919,6 +3039,11 @@
       <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr"/>
       <c r="AG25" t="inlineStr"/>
+      <c r="AH25" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2951,7 +3076,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -3008,6 +3133,11 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" t="inlineStr"/>
       <c r="AG26" t="inlineStr"/>
+      <c r="AH26" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3040,7 +3170,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Kanban</t>
+          <t>['Kanban']</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -3117,6 +3247,11 @@
       <c r="AE27" t="inlineStr"/>
       <c r="AF27" t="inlineStr"/>
       <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr">
+        <is>
+          <t>['Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3149,7 +3284,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Kanban, Lean</t>
+          <t>['Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -3198,6 +3333,11 @@
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr"/>
       <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr">
+        <is>
+          <t>['Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3230,7 +3370,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -3295,6 +3435,11 @@
       <c r="AE29" t="inlineStr"/>
       <c r="AF29" t="inlineStr"/>
       <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3327,7 +3472,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
@@ -3359,7 +3504,7 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Delivery to customer, Number of Active Customers, NPS</t>
+          <t>Number of Active Customers, NPS</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3396,6 +3541,11 @@
       <c r="AE30" t="inlineStr"/>
       <c r="AF30" t="inlineStr"/>
       <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3428,7 +3578,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -3485,6 +3635,11 @@
       <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr"/>
       <c r="AG31" t="inlineStr"/>
+      <c r="AH31" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3517,7 +3672,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -3586,6 +3741,11 @@
       <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr"/>
       <c r="AG32" t="inlineStr"/>
+      <c r="AH32" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3618,7 +3778,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -3679,6 +3839,11 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" t="inlineStr"/>
       <c r="AG33" t="inlineStr"/>
+      <c r="AH33" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3711,7 +3876,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean, Lean Inception, iniciando praticas no AUF (Agile Upstream Framework)</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H34" t="inlineStr"/>
@@ -3768,6 +3933,11 @@
       <c r="AE34" t="inlineStr"/>
       <c r="AF34" t="inlineStr"/>
       <c r="AG34" t="inlineStr"/>
+      <c r="AH34" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean', 'Lean Inception', 'iniciando praticas no AUF (Agile Upstream Framework)']</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3800,7 +3970,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Safe</t>
+          <t>['Scrum', 'Kanban', 'Safe']</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -3873,6 +4043,11 @@
       <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr"/>
       <c r="AG35" t="inlineStr"/>
+      <c r="AH35" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Safe']</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3905,7 +4080,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -3966,6 +4141,11 @@
       <c r="AE36" t="inlineStr"/>
       <c r="AF36" t="inlineStr"/>
       <c r="AG36" t="inlineStr"/>
+      <c r="AH36" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3998,7 +4178,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Scrum, Lean</t>
+          <t>['Scrum', 'Lean']</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -4055,6 +4235,11 @@
       <c r="AE37" t="inlineStr"/>
       <c r="AF37" t="inlineStr"/>
       <c r="AG37" t="inlineStr"/>
+      <c r="AH37" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4087,7 +4272,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Kanban, Safe</t>
+          <t>['Kanban', 'Safe']</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -4144,6 +4329,11 @@
       <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr"/>
       <c r="AG38" t="inlineStr"/>
+      <c r="AH38" t="inlineStr">
+        <is>
+          <t>['Kanban', 'Safe']</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4176,7 +4366,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -4233,6 +4423,11 @@
       <c r="AE39" t="inlineStr"/>
       <c r="AF39" t="inlineStr"/>
       <c r="AG39" t="inlineStr"/>
+      <c r="AH39" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4265,7 +4460,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -4318,6 +4513,11 @@
       <c r="AE40" t="inlineStr"/>
       <c r="AF40" t="inlineStr"/>
       <c r="AG40" t="inlineStr"/>
+      <c r="AH40" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4346,7 +4546,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Scrum, Híbrido </t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -4411,6 +4611,11 @@
       <c r="AE41" t="inlineStr"/>
       <c r="AF41" t="inlineStr"/>
       <c r="AG41" t="inlineStr"/>
+      <c r="AH41" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Híbrido ']</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4439,7 +4644,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
@@ -4480,6 +4685,11 @@
       <c r="AE42" t="inlineStr"/>
       <c r="AF42" t="inlineStr"/>
       <c r="AG42" t="inlineStr"/>
+      <c r="AH42" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4512,7 +4722,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Scrum, XP</t>
+          <t>['Scrum', 'XP']</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -4569,6 +4779,11 @@
       <c r="AE43" t="inlineStr"/>
       <c r="AF43" t="inlineStr"/>
       <c r="AG43" t="inlineStr"/>
+      <c r="AH43" t="inlineStr">
+        <is>
+          <t>['Scrum', 'XP']</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4601,7 +4816,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H44" t="inlineStr"/>
@@ -4654,6 +4869,11 @@
       <c r="AE44" t="inlineStr"/>
       <c r="AF44" t="inlineStr"/>
       <c r="AG44" t="inlineStr"/>
+      <c r="AH44" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4686,7 +4906,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -4716,11 +4936,7 @@
           <t>Cronograma e progresso, Produto, Processo, Tecnologia</t>
         </is>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>Produto, Produto, Produto, Produto, Produto</t>
-        </is>
-      </c>
+      <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr">
         <is>
           <t>Produto</t>
@@ -4759,6 +4975,11 @@
       <c r="AE45" t="inlineStr"/>
       <c r="AF45" t="inlineStr"/>
       <c r="AG45" t="inlineStr"/>
+      <c r="AH45" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4791,7 +5012,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -4856,6 +5077,11 @@
       <c r="AE46" t="inlineStr"/>
       <c r="AF46" t="inlineStr"/>
       <c r="AG46" t="inlineStr"/>
+      <c r="AH46" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4888,7 +5114,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -4941,6 +5167,11 @@
       <c r="AE47" t="inlineStr"/>
       <c r="AF47" t="inlineStr"/>
       <c r="AG47" t="inlineStr"/>
+      <c r="AH47" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4973,7 +5204,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -5005,7 +5236,7 @@
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Lead time, Throughput, Cumulative Flow Diagrams, CFD, OKR</t>
+          <t>Lead time, Throughput, CFD, OKR</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -5046,6 +5277,11 @@
       <c r="AE48" t="inlineStr"/>
       <c r="AF48" t="inlineStr"/>
       <c r="AG48" t="inlineStr"/>
+      <c r="AH48" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -5078,7 +5314,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Kanban</t>
+          <t>['Kanban']</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -5110,7 +5346,7 @@
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Lead time, Throughput, Cumulative Flow Diagrams</t>
+          <t>Lead time, Throughput</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -5143,6 +5379,11 @@
       <c r="AE49" t="inlineStr"/>
       <c r="AF49" t="inlineStr"/>
       <c r="AG49" t="inlineStr"/>
+      <c r="AH49" t="inlineStr">
+        <is>
+          <t>['Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5175,7 +5416,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -5240,6 +5481,11 @@
       <c r="AE50" t="inlineStr"/>
       <c r="AF50" t="inlineStr"/>
       <c r="AG50" t="inlineStr"/>
+      <c r="AH50" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5272,7 +5518,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H51" t="inlineStr"/>
@@ -5341,6 +5587,11 @@
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" t="inlineStr"/>
       <c r="AG51" t="inlineStr"/>
+      <c r="AH51" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5373,7 +5624,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -5446,6 +5697,11 @@
       <c r="AE52" t="inlineStr"/>
       <c r="AF52" t="inlineStr"/>
       <c r="AG52" t="inlineStr"/>
+      <c r="AH52" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5478,7 +5734,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
@@ -5523,6 +5779,11 @@
       <c r="AE53" t="inlineStr"/>
       <c r="AF53" t="inlineStr"/>
       <c r="AG53" t="inlineStr"/>
+      <c r="AH53" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -5555,7 +5816,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -5620,6 +5881,11 @@
       <c r="AE54" t="inlineStr"/>
       <c r="AF54" t="inlineStr"/>
       <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -5652,7 +5918,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -5721,6 +5987,11 @@
       <c r="AE55" t="inlineStr"/>
       <c r="AF55" t="inlineStr"/>
       <c r="AG55" t="inlineStr"/>
+      <c r="AH55" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -5753,7 +6024,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>ScrumBan, Kanban, Adaptação de Kanban e Scrum a nossa realidade</t>
+          <t>['ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -5785,7 +6056,7 @@
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Throughput, Team total available hours, Velocity, Horas extras</t>
+          <t>Throughput, Team total available hours, Velocity</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -5822,6 +6093,11 @@
       <c r="AE56" t="inlineStr"/>
       <c r="AF56" t="inlineStr"/>
       <c r="AG56" t="inlineStr"/>
+      <c r="AH56" t="inlineStr">
+        <is>
+          <t>['ScrumBan', 'Kanban', 'Adaptação de Kanban e Scrum a nossa realidade']</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -5854,7 +6130,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -5919,6 +6195,11 @@
       <c r="AE57" t="inlineStr"/>
       <c r="AF57" t="inlineStr"/>
       <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -5951,7 +6232,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -6012,6 +6293,11 @@
       <c r="AE58" t="inlineStr"/>
       <c r="AF58" t="inlineStr"/>
       <c r="AG58" t="inlineStr"/>
+      <c r="AH58" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -6044,7 +6330,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -6097,6 +6383,11 @@
       <c r="AE59" t="inlineStr"/>
       <c r="AF59" t="inlineStr"/>
       <c r="AG59" t="inlineStr"/>
+      <c r="AH59" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -6129,7 +6420,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
@@ -6178,6 +6469,11 @@
       <c r="AE60" t="inlineStr"/>
       <c r="AF60" t="inlineStr"/>
       <c r="AG60" t="inlineStr"/>
+      <c r="AH60" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -6210,7 +6506,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
@@ -6271,6 +6567,11 @@
       <c r="AE61" t="inlineStr"/>
       <c r="AF61" t="inlineStr"/>
       <c r="AG61" t="inlineStr"/>
+      <c r="AH61" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -6303,7 +6604,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -6368,6 +6669,11 @@
       <c r="AE62" t="inlineStr"/>
       <c r="AF62" t="inlineStr"/>
       <c r="AG62" t="inlineStr"/>
+      <c r="AH62" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6400,7 +6706,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -6469,6 +6775,11 @@
       <c r="AE63" t="inlineStr"/>
       <c r="AF63" t="inlineStr"/>
       <c r="AG63" t="inlineStr"/>
+      <c r="AH63" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -6501,7 +6812,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -6546,6 +6857,11 @@
       <c r="AE64" t="inlineStr"/>
       <c r="AF64" t="inlineStr"/>
       <c r="AG64" t="inlineStr"/>
+      <c r="AH64" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -6578,7 +6894,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H65" t="inlineStr"/>
@@ -6635,6 +6951,11 @@
       <c r="AE65" t="inlineStr"/>
       <c r="AF65" t="inlineStr"/>
       <c r="AG65" t="inlineStr"/>
+      <c r="AH65" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -6667,7 +6988,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
@@ -6736,6 +7057,11 @@
       <c r="AE66" t="inlineStr"/>
       <c r="AF66" t="inlineStr"/>
       <c r="AG66" t="inlineStr"/>
+      <c r="AH66" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -6768,7 +7094,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -6821,6 +7147,11 @@
       <c r="AE67" t="inlineStr"/>
       <c r="AF67" t="inlineStr"/>
       <c r="AG67" t="inlineStr"/>
+      <c r="AH67" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -6853,7 +7184,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -6926,6 +7257,11 @@
       <c r="AE68" t="inlineStr"/>
       <c r="AF68" t="inlineStr"/>
       <c r="AG68" t="inlineStr"/>
+      <c r="AH68" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6958,7 +7294,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>ScrumBan, Kanban</t>
+          <t>['ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
@@ -7019,6 +7355,11 @@
       <c r="AE69" t="inlineStr"/>
       <c r="AF69" t="inlineStr"/>
       <c r="AG69" t="inlineStr"/>
+      <c r="AH69" t="inlineStr">
+        <is>
+          <t>['ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -7051,7 +7392,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -7104,6 +7445,11 @@
       <c r="AE70" t="inlineStr"/>
       <c r="AF70" t="inlineStr"/>
       <c r="AG70" t="inlineStr"/>
+      <c r="AH70" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -7136,7 +7482,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -7201,6 +7547,11 @@
       <c r="AE71" t="inlineStr"/>
       <c r="AF71" t="inlineStr"/>
       <c r="AG71" t="inlineStr"/>
+      <c r="AH71" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -7229,7 +7580,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -7298,6 +7649,11 @@
       <c r="AE72" t="inlineStr"/>
       <c r="AF72" t="inlineStr"/>
       <c r="AG72" t="inlineStr"/>
+      <c r="AH72" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -7330,7 +7686,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Kanban</t>
+          <t>['Kanban']</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
@@ -7387,6 +7743,11 @@
       <c r="AE73" t="inlineStr"/>
       <c r="AF73" t="inlineStr"/>
       <c r="AG73" t="inlineStr"/>
+      <c r="AH73" t="inlineStr">
+        <is>
+          <t>['Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -7419,7 +7780,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Kanban</t>
+          <t>['Kanban']</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -7468,6 +7829,11 @@
       <c r="AE74" t="inlineStr"/>
       <c r="AF74" t="inlineStr"/>
       <c r="AG74" t="inlineStr"/>
+      <c r="AH74" t="inlineStr">
+        <is>
+          <t>['Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -7500,7 +7866,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
@@ -7553,6 +7919,11 @@
       <c r="AE75" t="inlineStr"/>
       <c r="AF75" t="inlineStr"/>
       <c r="AG75" t="inlineStr"/>
+      <c r="AH75" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -7585,7 +7956,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
@@ -7642,6 +8013,11 @@
       <c r="AE76" t="inlineStr"/>
       <c r="AF76" t="inlineStr"/>
       <c r="AG76" t="inlineStr"/>
+      <c r="AH76" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -7674,7 +8050,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -7739,6 +8115,11 @@
       <c r="AE77" t="inlineStr"/>
       <c r="AF77" t="inlineStr"/>
       <c r="AG77" t="inlineStr"/>
+      <c r="AH77" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -7771,7 +8152,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Kanban, Lean</t>
+          <t>['Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -7840,6 +8221,11 @@
       <c r="AE78" t="inlineStr"/>
       <c r="AF78" t="inlineStr"/>
       <c r="AG78" t="inlineStr"/>
+      <c r="AH78" t="inlineStr">
+        <is>
+          <t>['Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -7872,7 +8258,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Scrum, Lean</t>
+          <t>['Scrum', 'Lean']</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -7925,6 +8311,11 @@
       <c r="AE79" t="inlineStr"/>
       <c r="AF79" t="inlineStr"/>
       <c r="AG79" t="inlineStr"/>
+      <c r="AH79" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -7957,7 +8348,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -8018,6 +8409,11 @@
       <c r="AE80" t="inlineStr"/>
       <c r="AF80" t="inlineStr"/>
       <c r="AG80" t="inlineStr"/>
+      <c r="AH80" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -8050,7 +8446,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
@@ -8099,6 +8495,11 @@
       <c r="AE81" t="inlineStr"/>
       <c r="AF81" t="inlineStr"/>
       <c r="AG81" t="inlineStr"/>
+      <c r="AH81" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -8131,7 +8532,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
@@ -8188,6 +8589,11 @@
       <c r="AE82" t="inlineStr"/>
       <c r="AF82" t="inlineStr"/>
       <c r="AG82" t="inlineStr"/>
+      <c r="AH82" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -8220,7 +8626,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
@@ -8277,6 +8683,11 @@
       <c r="AE83" t="inlineStr"/>
       <c r="AF83" t="inlineStr"/>
       <c r="AG83" t="inlineStr"/>
+      <c r="AH83" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -8309,7 +8720,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
@@ -8333,7 +8744,7 @@
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Delivery to customer, Conversão, Conversão</t>
+          <t>Conversão, Conversão</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -8370,6 +8781,11 @@
       <c r="AE84" t="inlineStr"/>
       <c r="AF84" t="inlineStr"/>
       <c r="AG84" t="inlineStr"/>
+      <c r="AH84" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -8402,7 +8818,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>ScrumBan, Lean</t>
+          <t>['ScrumBan', 'Lean']</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
@@ -8459,6 +8875,11 @@
       <c r="AE85" t="inlineStr"/>
       <c r="AF85" t="inlineStr"/>
       <c r="AG85" t="inlineStr"/>
+      <c r="AH85" t="inlineStr">
+        <is>
+          <t>['ScrumBan', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -8491,7 +8912,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
@@ -8511,7 +8932,7 @@
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Ideal team capacity, Cumulative Flow Diagrams, Velocity, Quality rating</t>
+          <t>Ideal team capacity, Velocity, Quality rating</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -8552,6 +8973,11 @@
       <c r="AE86" t="inlineStr"/>
       <c r="AF86" t="inlineStr"/>
       <c r="AG86" t="inlineStr"/>
+      <c r="AH86" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -8584,7 +9010,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -8641,6 +9067,11 @@
       <c r="AE87" t="inlineStr"/>
       <c r="AF87" t="inlineStr"/>
       <c r="AG87" t="inlineStr"/>
+      <c r="AH87" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -8673,7 +9104,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
@@ -8742,6 +9173,11 @@
       <c r="AE88" t="inlineStr"/>
       <c r="AF88" t="inlineStr"/>
       <c r="AG88" t="inlineStr"/>
+      <c r="AH88" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -8774,7 +9210,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -8839,6 +9275,11 @@
       <c r="AE89" t="inlineStr"/>
       <c r="AF89" t="inlineStr"/>
       <c r="AG89" t="inlineStr"/>
+      <c r="AH89" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -8871,7 +9312,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -8932,6 +9373,11 @@
       <c r="AE90" t="inlineStr"/>
       <c r="AF90" t="inlineStr"/>
       <c r="AG90" t="inlineStr"/>
+      <c r="AH90" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -8964,7 +9410,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -9033,6 +9479,11 @@
       <c r="AE91" t="inlineStr"/>
       <c r="AF91" t="inlineStr"/>
       <c r="AG91" t="inlineStr"/>
+      <c r="AH91" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -9065,7 +9516,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -9142,6 +9593,11 @@
       <c r="AE92" t="inlineStr"/>
       <c r="AF92" t="inlineStr"/>
       <c r="AG92" t="inlineStr"/>
+      <c r="AH92" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -9174,7 +9630,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -9243,6 +9699,11 @@
       <c r="AE93" t="inlineStr"/>
       <c r="AF93" t="inlineStr"/>
       <c r="AG93" t="inlineStr"/>
+      <c r="AH93" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -9275,7 +9736,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
@@ -9324,6 +9785,11 @@
       <c r="AE94" t="inlineStr"/>
       <c r="AF94" t="inlineStr"/>
       <c r="AG94" t="inlineStr"/>
+      <c r="AH94" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -9356,7 +9822,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Kanban, Lean</t>
+          <t>['Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
@@ -9405,6 +9871,11 @@
       <c r="AE95" t="inlineStr"/>
       <c r="AF95" t="inlineStr"/>
       <c r="AG95" t="inlineStr"/>
+      <c r="AH95" t="inlineStr">
+        <is>
+          <t>['Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -9437,7 +9908,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
@@ -9494,6 +9965,11 @@
       <c r="AE96" t="inlineStr"/>
       <c r="AF96" t="inlineStr"/>
       <c r="AG96" t="inlineStr"/>
+      <c r="AH96" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -9526,7 +10002,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -9587,6 +10063,11 @@
       <c r="AE97" t="inlineStr"/>
       <c r="AF97" t="inlineStr"/>
       <c r="AG97" t="inlineStr"/>
+      <c r="AH97" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -9619,7 +10100,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
@@ -9688,6 +10169,11 @@
       <c r="AE98" t="inlineStr"/>
       <c r="AF98" t="inlineStr"/>
       <c r="AG98" t="inlineStr"/>
+      <c r="AH98" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -9720,7 +10206,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
@@ -9769,6 +10255,11 @@
       <c r="AE99" t="inlineStr"/>
       <c r="AF99" t="inlineStr"/>
       <c r="AG99" t="inlineStr"/>
+      <c r="AH99" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -9801,7 +10292,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -9858,6 +10349,11 @@
       <c r="AE100" t="inlineStr"/>
       <c r="AF100" t="inlineStr"/>
       <c r="AG100" t="inlineStr"/>
+      <c r="AH100" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -9890,7 +10386,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
@@ -9963,6 +10459,11 @@
       <c r="AE101" t="inlineStr"/>
       <c r="AF101" t="inlineStr"/>
       <c r="AG101" t="inlineStr"/>
+      <c r="AH101" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -9995,7 +10496,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Scrum, XP, Kanban, Lean</t>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -10052,6 +10553,11 @@
       <c r="AE102" t="inlineStr"/>
       <c r="AF102" t="inlineStr"/>
       <c r="AG102" t="inlineStr"/>
+      <c r="AH102" t="inlineStr">
+        <is>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -10084,7 +10590,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -10145,6 +10651,11 @@
       <c r="AE103" t="inlineStr"/>
       <c r="AF103" t="inlineStr"/>
       <c r="AG103" t="inlineStr"/>
+      <c r="AH103" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -10177,7 +10688,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -10242,6 +10753,11 @@
       <c r="AE104" t="inlineStr"/>
       <c r="AF104" t="inlineStr"/>
       <c r="AG104" t="inlineStr"/>
+      <c r="AH104" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -10274,7 +10790,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
@@ -10327,6 +10843,11 @@
       <c r="AE105" t="inlineStr"/>
       <c r="AF105" t="inlineStr"/>
       <c r="AG105" t="inlineStr"/>
+      <c r="AH105" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -10359,7 +10880,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Kanban, Lean</t>
+          <t>['Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -10424,6 +10945,11 @@
       <c r="AE106" t="inlineStr"/>
       <c r="AF106" t="inlineStr"/>
       <c r="AG106" t="inlineStr"/>
+      <c r="AH106" t="inlineStr">
+        <is>
+          <t>['Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -10456,7 +10982,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Scrum, XP, Kanban, Lean</t>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H107" t="inlineStr"/>
@@ -10505,6 +11031,11 @@
       <c r="AE107" t="inlineStr"/>
       <c r="AF107" t="inlineStr"/>
       <c r="AG107" t="inlineStr"/>
+      <c r="AH107" t="inlineStr">
+        <is>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -10537,7 +11068,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>XP, Kanban</t>
+          <t>['XP', 'Kanban']</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
@@ -10594,6 +11125,11 @@
       <c r="AE108" t="inlineStr"/>
       <c r="AF108" t="inlineStr"/>
       <c r="AG108" t="inlineStr"/>
+      <c r="AH108" t="inlineStr">
+        <is>
+          <t>['XP', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -10626,7 +11162,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -10691,6 +11227,11 @@
       <c r="AE109" t="inlineStr"/>
       <c r="AF109" t="inlineStr"/>
       <c r="AG109" t="inlineStr"/>
+      <c r="AH109" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -10723,7 +11264,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -10800,6 +11341,11 @@
       <c r="AE110" t="inlineStr"/>
       <c r="AF110" t="inlineStr"/>
       <c r="AG110" t="inlineStr"/>
+      <c r="AH110" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -10832,7 +11378,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -10860,7 +11406,7 @@
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>Horas extras, Cycle time, Horas extras, Cycle time</t>
+          <t>Cycle time, Cycle time</t>
         </is>
       </c>
       <c r="P111" t="inlineStr">
@@ -10897,6 +11443,11 @@
       <c r="AE111" t="inlineStr"/>
       <c r="AF111" t="inlineStr"/>
       <c r="AG111" t="inlineStr"/>
+      <c r="AH111" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -10929,7 +11480,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean, Safe</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean', 'Safe']</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -10998,6 +11549,11 @@
       <c r="AE112" t="inlineStr"/>
       <c r="AF112" t="inlineStr"/>
       <c r="AG112" t="inlineStr"/>
+      <c r="AH112" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean', 'Safe']</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -11030,7 +11586,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -11087,6 +11643,11 @@
       <c r="AE113" t="inlineStr"/>
       <c r="AF113" t="inlineStr"/>
       <c r="AG113" t="inlineStr"/>
+      <c r="AH113" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -11119,7 +11680,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -11184,6 +11745,11 @@
       <c r="AE114" t="inlineStr"/>
       <c r="AF114" t="inlineStr"/>
       <c r="AG114" t="inlineStr"/>
+      <c r="AH114" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -11216,7 +11782,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
@@ -11281,6 +11847,11 @@
       <c r="AE115" t="inlineStr"/>
       <c r="AF115" t="inlineStr"/>
       <c r="AG115" t="inlineStr"/>
+      <c r="AH115" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -11313,7 +11884,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H116" t="inlineStr"/>
@@ -11366,6 +11937,11 @@
       <c r="AE116" t="inlineStr"/>
       <c r="AF116" t="inlineStr"/>
       <c r="AG116" t="inlineStr"/>
+      <c r="AH116" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -11398,7 +11974,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
@@ -11459,6 +12035,11 @@
       <c r="AE117" t="inlineStr"/>
       <c r="AF117" t="inlineStr"/>
       <c r="AG117" t="inlineStr"/>
+      <c r="AH117" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -11491,7 +12072,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
@@ -11536,6 +12117,11 @@
       <c r="AE118" t="inlineStr"/>
       <c r="AF118" t="inlineStr"/>
       <c r="AG118" t="inlineStr"/>
+      <c r="AH118" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -11564,7 +12150,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H119" t="inlineStr"/>
@@ -11637,6 +12223,11 @@
       <c r="AE119" t="inlineStr"/>
       <c r="AF119" t="inlineStr"/>
       <c r="AG119" t="inlineStr"/>
+      <c r="AH119" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -11669,7 +12260,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
@@ -11722,6 +12313,11 @@
       <c r="AE120" t="inlineStr"/>
       <c r="AF120" t="inlineStr"/>
       <c r="AG120" t="inlineStr"/>
+      <c r="AH120" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -11754,7 +12350,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -11827,6 +12423,11 @@
       <c r="AE121" t="inlineStr"/>
       <c r="AF121" t="inlineStr"/>
       <c r="AG121" t="inlineStr"/>
+      <c r="AH121" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -11859,7 +12460,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H122" t="inlineStr"/>
@@ -11908,6 +12509,11 @@
       <c r="AE122" t="inlineStr"/>
       <c r="AF122" t="inlineStr"/>
       <c r="AG122" t="inlineStr"/>
+      <c r="AH122" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -11940,7 +12546,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -11972,7 +12578,7 @@
       </c>
       <c r="O123" t="inlineStr">
         <is>
-          <t>Clima, Project avg. cost, Project avg. cost, Technical Efficiency, Ideal team capacity, SLA, Test Coverage, Lead time, Cycle time, NPS, Conversão, Conversão, Conversão, Number of completed tasks, User Story Points</t>
+          <t>Project avg. cost, Project avg. cost, Technical Efficiency, Ideal team capacity, SLA, Test Coverage, Lead time, Cycle time, NPS, Conversão, Conversão, Conversão, Number of completed tasks, User Story Points</t>
         </is>
       </c>
       <c r="P123" t="inlineStr">
@@ -12063,6 +12669,11 @@
       <c r="AG123" t="inlineStr">
         <is>
           <t>User Story Points</t>
+        </is>
+      </c>
+      <c r="AH123" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
     </row>
@@ -12097,7 +12708,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -12162,6 +12773,11 @@
       <c r="AE124" t="inlineStr"/>
       <c r="AF124" t="inlineStr"/>
       <c r="AG124" t="inlineStr"/>
+      <c r="AH124" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -12194,7 +12810,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H125" t="inlineStr"/>
@@ -12243,6 +12859,11 @@
       <c r="AE125" t="inlineStr"/>
       <c r="AF125" t="inlineStr"/>
       <c r="AG125" t="inlineStr"/>
+      <c r="AH125" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -12275,7 +12896,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t xml:space="preserve">XP, Kanban, Lean, Fluxo unificado </t>
+          <t>['XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H126" t="inlineStr"/>
@@ -12340,6 +12961,11 @@
       <c r="AE126" t="inlineStr"/>
       <c r="AF126" t="inlineStr"/>
       <c r="AG126" t="inlineStr"/>
+      <c r="AH126" t="inlineStr">
+        <is>
+          <t>['XP', 'Kanban', 'Lean', 'Fluxo unificado ']</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -12372,7 +12998,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
@@ -12425,6 +13051,11 @@
       <c r="AE127" t="inlineStr"/>
       <c r="AF127" t="inlineStr"/>
       <c r="AG127" t="inlineStr"/>
+      <c r="AH127" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -12457,7 +13088,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H128" t="inlineStr"/>
@@ -12514,6 +13145,11 @@
       <c r="AE128" t="inlineStr"/>
       <c r="AF128" t="inlineStr"/>
       <c r="AG128" t="inlineStr"/>
+      <c r="AH128" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -12546,7 +13182,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H129" t="inlineStr"/>
@@ -12607,6 +13243,11 @@
       <c r="AE129" t="inlineStr"/>
       <c r="AF129" t="inlineStr"/>
       <c r="AG129" t="inlineStr"/>
+      <c r="AH129" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -12639,7 +13280,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
@@ -12704,6 +13345,11 @@
       <c r="AE130" t="inlineStr"/>
       <c r="AF130" t="inlineStr"/>
       <c r="AG130" t="inlineStr"/>
+      <c r="AH130" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -12736,7 +13382,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -12764,7 +13410,7 @@
       </c>
       <c r="O131" t="inlineStr">
         <is>
-          <t>CAC, Lead time, Cycle time, Burndown, Delivery to customer</t>
+          <t>CAC, Lead time, Cycle time, Burndown</t>
         </is>
       </c>
       <c r="P131" t="inlineStr">
@@ -12805,6 +13451,11 @@
       <c r="AE131" t="inlineStr"/>
       <c r="AF131" t="inlineStr"/>
       <c r="AG131" t="inlineStr"/>
+      <c r="AH131" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -12837,7 +13488,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -12910,6 +13561,11 @@
       <c r="AE132" t="inlineStr"/>
       <c r="AF132" t="inlineStr"/>
       <c r="AG132" t="inlineStr"/>
+      <c r="AH132" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -12942,7 +13598,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -13007,6 +13663,11 @@
       <c r="AE133" t="inlineStr"/>
       <c r="AF133" t="inlineStr"/>
       <c r="AG133" t="inlineStr"/>
+      <c r="AH133" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -13039,7 +13700,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Scrum, XP, Kanban, Lean</t>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -13088,6 +13749,11 @@
       <c r="AE134" t="inlineStr"/>
       <c r="AF134" t="inlineStr"/>
       <c r="AG134" t="inlineStr"/>
+      <c r="AH134" t="inlineStr">
+        <is>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -13120,7 +13786,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H135" t="inlineStr"/>
@@ -13140,7 +13806,7 @@
       </c>
       <c r="O135" t="inlineStr">
         <is>
-          <t>Roadmaps, Team total available hours, Quality rating, Clima</t>
+          <t>Roadmaps, Team total available hours, Quality rating</t>
         </is>
       </c>
       <c r="P135" t="inlineStr">
@@ -13177,6 +13843,11 @@
       <c r="AE135" t="inlineStr"/>
       <c r="AF135" t="inlineStr"/>
       <c r="AG135" t="inlineStr"/>
+      <c r="AH135" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -13209,7 +13880,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -13278,6 +13949,11 @@
       <c r="AE136" t="inlineStr"/>
       <c r="AF136" t="inlineStr"/>
       <c r="AG136" t="inlineStr"/>
+      <c r="AH136" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -13310,7 +13986,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H137" t="inlineStr"/>
@@ -13363,6 +14039,11 @@
       <c r="AE137" t="inlineStr"/>
       <c r="AF137" t="inlineStr"/>
       <c r="AG137" t="inlineStr"/>
+      <c r="AH137" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -13395,7 +14076,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
@@ -13464,6 +14145,11 @@
       <c r="AE138" t="inlineStr"/>
       <c r="AF138" t="inlineStr"/>
       <c r="AG138" t="inlineStr"/>
+      <c r="AH138" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -13496,7 +14182,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan</t>
+          <t>['Scrum', 'ScrumBan']</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
@@ -13516,7 +14202,7 @@
       </c>
       <c r="O139" t="inlineStr">
         <is>
-          <t>Clima, Dívidas técnicas, Project avg. cost</t>
+          <t>Dívidas técnicas, Project avg. cost</t>
         </is>
       </c>
       <c r="P139" t="inlineStr">
@@ -13557,6 +14243,11 @@
       <c r="AE139" t="inlineStr"/>
       <c r="AF139" t="inlineStr"/>
       <c r="AG139" t="inlineStr"/>
+      <c r="AH139" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -13589,7 +14280,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H140" t="inlineStr"/>
@@ -13654,6 +14345,11 @@
       <c r="AE140" t="inlineStr"/>
       <c r="AF140" t="inlineStr"/>
       <c r="AG140" t="inlineStr"/>
+      <c r="AH140" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -13686,7 +14382,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H141" t="inlineStr"/>
@@ -13743,6 +14439,11 @@
       <c r="AE141" t="inlineStr"/>
       <c r="AF141" t="inlineStr"/>
       <c r="AG141" t="inlineStr"/>
+      <c r="AH141" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -13775,7 +14476,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -13828,6 +14529,11 @@
       <c r="AE142" t="inlineStr"/>
       <c r="AF142" t="inlineStr"/>
       <c r="AG142" t="inlineStr"/>
+      <c r="AH142" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -13860,7 +14566,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H143" t="inlineStr"/>
@@ -13921,6 +14627,11 @@
       <c r="AE143" t="inlineStr"/>
       <c r="AF143" t="inlineStr"/>
       <c r="AG143" t="inlineStr"/>
+      <c r="AH143" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -13953,7 +14664,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H144" t="inlineStr"/>
@@ -14018,6 +14729,11 @@
       <c r="AE144" t="inlineStr"/>
       <c r="AF144" t="inlineStr"/>
       <c r="AG144" t="inlineStr"/>
+      <c r="AH144" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -14050,7 +14766,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H145" t="inlineStr"/>
@@ -14099,6 +14815,11 @@
       <c r="AE145" t="inlineStr"/>
       <c r="AF145" t="inlineStr"/>
       <c r="AG145" t="inlineStr"/>
+      <c r="AH145" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -14131,7 +14852,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H146" t="inlineStr"/>
@@ -14192,6 +14913,11 @@
       <c r="AE146" t="inlineStr"/>
       <c r="AF146" t="inlineStr"/>
       <c r="AG146" t="inlineStr"/>
+      <c r="AH146" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -14224,7 +14950,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -14285,6 +15011,11 @@
       <c r="AE147" t="inlineStr"/>
       <c r="AF147" t="inlineStr"/>
       <c r="AG147" t="inlineStr"/>
+      <c r="AH147" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -14317,7 +15048,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
@@ -14370,6 +15101,11 @@
       <c r="AE148" t="inlineStr"/>
       <c r="AF148" t="inlineStr"/>
       <c r="AG148" t="inlineStr"/>
+      <c r="AH148" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -14402,7 +15138,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Kanban</t>
+          <t>['Kanban']</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
@@ -14471,6 +15207,11 @@
       <c r="AE149" t="inlineStr"/>
       <c r="AF149" t="inlineStr"/>
       <c r="AG149" t="inlineStr"/>
+      <c r="AH149" t="inlineStr">
+        <is>
+          <t>['Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -14503,7 +15244,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -14580,6 +15321,11 @@
       <c r="AE150" t="inlineStr"/>
       <c r="AF150" t="inlineStr"/>
       <c r="AG150" t="inlineStr"/>
+      <c r="AH150" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -14612,7 +15358,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -14677,6 +15423,11 @@
       <c r="AE151" t="inlineStr"/>
       <c r="AF151" t="inlineStr"/>
       <c r="AG151" t="inlineStr"/>
+      <c r="AH151" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -14709,7 +15460,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H152" t="inlineStr"/>
@@ -14754,6 +15505,11 @@
       <c r="AE152" t="inlineStr"/>
       <c r="AF152" t="inlineStr"/>
       <c r="AG152" t="inlineStr"/>
+      <c r="AH152" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -14786,7 +15542,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
@@ -14863,6 +15619,11 @@
       <c r="AE153" t="inlineStr"/>
       <c r="AF153" t="inlineStr"/>
       <c r="AG153" t="inlineStr"/>
+      <c r="AH153" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -14895,7 +15656,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
@@ -14956,6 +15717,11 @@
       <c r="AE154" t="inlineStr"/>
       <c r="AF154" t="inlineStr"/>
       <c r="AG154" t="inlineStr"/>
+      <c r="AH154" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -14988,7 +15754,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Kanban, Lean</t>
+          <t>['Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
@@ -15057,6 +15823,11 @@
       <c r="AE155" t="inlineStr"/>
       <c r="AF155" t="inlineStr"/>
       <c r="AG155" t="inlineStr"/>
+      <c r="AH155" t="inlineStr">
+        <is>
+          <t>['Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -15089,7 +15860,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H156" t="inlineStr"/>
@@ -15134,6 +15905,11 @@
       <c r="AE156" t="inlineStr"/>
       <c r="AF156" t="inlineStr"/>
       <c r="AG156" t="inlineStr"/>
+      <c r="AH156" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -15166,7 +15942,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
@@ -15235,6 +16011,11 @@
       <c r="AE157" t="inlineStr"/>
       <c r="AF157" t="inlineStr"/>
       <c r="AG157" t="inlineStr"/>
+      <c r="AH157" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -15267,7 +16048,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
@@ -15332,6 +16113,11 @@
       <c r="AE158" t="inlineStr"/>
       <c r="AF158" t="inlineStr"/>
       <c r="AG158" t="inlineStr"/>
+      <c r="AH158" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -15364,7 +16150,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -15429,6 +16215,11 @@
       <c r="AE159" t="inlineStr"/>
       <c r="AF159" t="inlineStr"/>
       <c r="AG159" t="inlineStr"/>
+      <c r="AH159" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -15461,7 +16252,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -15506,6 +16297,11 @@
       <c r="AE160" t="inlineStr"/>
       <c r="AF160" t="inlineStr"/>
       <c r="AG160" t="inlineStr"/>
+      <c r="AH160" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -15538,7 +16334,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Scrum, XP, Kanban</t>
+          <t>['Scrum', 'XP', 'Kanban']</t>
         </is>
       </c>
       <c r="H161" t="inlineStr"/>
@@ -15570,7 +16366,7 @@
       </c>
       <c r="O161" t="inlineStr">
         <is>
-          <t>Horas extras, Cycle time</t>
+          <t>Cycle time</t>
         </is>
       </c>
       <c r="P161" t="inlineStr">
@@ -15599,6 +16395,11 @@
       <c r="AE161" t="inlineStr"/>
       <c r="AF161" t="inlineStr"/>
       <c r="AG161" t="inlineStr"/>
+      <c r="AH161" t="inlineStr">
+        <is>
+          <t>['Scrum', 'XP', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -15631,7 +16432,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H162" t="inlineStr"/>
@@ -15696,6 +16497,11 @@
       <c r="AE162" t="inlineStr"/>
       <c r="AF162" t="inlineStr"/>
       <c r="AG162" t="inlineStr"/>
+      <c r="AH162" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -15728,7 +16534,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H163" t="inlineStr"/>
@@ -15789,6 +16595,11 @@
       <c r="AE163" t="inlineStr"/>
       <c r="AF163" t="inlineStr"/>
       <c r="AG163" t="inlineStr"/>
+      <c r="AH163" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -15821,7 +16632,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan</t>
+          <t>['Scrum', 'ScrumBan']</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
@@ -15878,6 +16689,11 @@
       <c r="AE164" t="inlineStr"/>
       <c r="AF164" t="inlineStr"/>
       <c r="AG164" t="inlineStr"/>
+      <c r="AH164" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -15910,7 +16726,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
@@ -15971,6 +16787,11 @@
       <c r="AE165" t="inlineStr"/>
       <c r="AF165" t="inlineStr"/>
       <c r="AG165" t="inlineStr"/>
+      <c r="AH165" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -16003,7 +16824,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -16072,6 +16893,11 @@
       <c r="AE166" t="inlineStr"/>
       <c r="AF166" t="inlineStr"/>
       <c r="AG166" t="inlineStr"/>
+      <c r="AH166" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -16104,7 +16930,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
@@ -16157,6 +16983,11 @@
       <c r="AE167" t="inlineStr"/>
       <c r="AF167" t="inlineStr"/>
       <c r="AG167" t="inlineStr"/>
+      <c r="AH167" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -16189,7 +17020,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -16246,6 +17077,11 @@
       <c r="AE168" t="inlineStr"/>
       <c r="AF168" t="inlineStr"/>
       <c r="AG168" t="inlineStr"/>
+      <c r="AH168" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -16278,7 +17114,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H169" t="inlineStr"/>
@@ -16347,6 +17183,11 @@
       <c r="AE169" t="inlineStr"/>
       <c r="AF169" t="inlineStr"/>
       <c r="AG169" t="inlineStr"/>
+      <c r="AH169" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -16379,7 +17220,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
@@ -16456,6 +17297,11 @@
       <c r="AE170" t="inlineStr"/>
       <c r="AF170" t="inlineStr"/>
       <c r="AG170" t="inlineStr"/>
+      <c r="AH170" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -16488,7 +17334,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -16545,6 +17391,11 @@
       <c r="AE171" t="inlineStr"/>
       <c r="AF171" t="inlineStr"/>
       <c r="AG171" t="inlineStr"/>
+      <c r="AH171" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -16577,7 +17428,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
@@ -16638,6 +17489,11 @@
       <c r="AE172" t="inlineStr"/>
       <c r="AF172" t="inlineStr"/>
       <c r="AG172" t="inlineStr"/>
+      <c r="AH172" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -16670,7 +17526,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Lean</t>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
@@ -16727,6 +17583,11 @@
       <c r="AE173" t="inlineStr"/>
       <c r="AF173" t="inlineStr"/>
       <c r="AG173" t="inlineStr"/>
+      <c r="AH173" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -16759,7 +17620,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Scrum, Kanban, Safe</t>
+          <t>['Scrum', 'Kanban', 'Safe']</t>
         </is>
       </c>
       <c r="H174" t="inlineStr">
@@ -16820,6 +17681,11 @@
       <c r="AE174" t="inlineStr"/>
       <c r="AF174" t="inlineStr"/>
       <c r="AG174" t="inlineStr"/>
+      <c r="AH174" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban', 'Safe']</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -16852,7 +17718,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Scrum, XP, Kanban</t>
+          <t>['Scrum', 'XP', 'Kanban']</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
@@ -16913,6 +17779,11 @@
       <c r="AE175" t="inlineStr"/>
       <c r="AF175" t="inlineStr"/>
       <c r="AG175" t="inlineStr"/>
+      <c r="AH175" t="inlineStr">
+        <is>
+          <t>['Scrum', 'XP', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -16945,7 +17816,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Scrum, XP, Kanban, Lean</t>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -17011,6 +17882,11 @@
       <c r="AE176" t="inlineStr"/>
       <c r="AF176" t="inlineStr"/>
       <c r="AG176" t="inlineStr"/>
+      <c r="AH176" t="inlineStr">
+        <is>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -17043,7 +17919,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -17100,6 +17976,11 @@
       <c r="AE177" t="inlineStr"/>
       <c r="AF177" t="inlineStr"/>
       <c r="AG177" t="inlineStr"/>
+      <c r="AH177" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -17132,7 +18013,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
@@ -17193,6 +18074,11 @@
       <c r="AE178" t="inlineStr"/>
       <c r="AF178" t="inlineStr"/>
       <c r="AG178" t="inlineStr"/>
+      <c r="AH178" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -17225,7 +18111,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
@@ -17278,6 +18164,11 @@
       <c r="AE179" t="inlineStr"/>
       <c r="AF179" t="inlineStr"/>
       <c r="AG179" t="inlineStr"/>
+      <c r="AH179" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -17310,7 +18201,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
@@ -17363,6 +18254,11 @@
       <c r="AE180" t="inlineStr"/>
       <c r="AF180" t="inlineStr"/>
       <c r="AG180" t="inlineStr"/>
+      <c r="AH180" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -17395,7 +18291,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -17460,6 +18356,11 @@
       <c r="AE181" t="inlineStr"/>
       <c r="AF181" t="inlineStr"/>
       <c r="AG181" t="inlineStr"/>
+      <c r="AH181" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -17488,7 +18389,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
@@ -17516,7 +18417,7 @@
       </c>
       <c r="O182" t="inlineStr">
         <is>
-          <t>Delivery to customer, Team total effective available hours, NPS, Quality rating, User Story Points</t>
+          <t>Team total effective available hours, NPS, Quality rating, User Story Points</t>
         </is>
       </c>
       <c r="P182" t="inlineStr">
@@ -17557,6 +18458,11 @@
       <c r="AE182" t="inlineStr"/>
       <c r="AF182" t="inlineStr"/>
       <c r="AG182" t="inlineStr"/>
+      <c r="AH182" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -17589,7 +18495,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan</t>
+          <t>['Scrum', 'ScrumBan']</t>
         </is>
       </c>
       <c r="H183" t="inlineStr"/>
@@ -17634,6 +18540,11 @@
       <c r="AE183" t="inlineStr"/>
       <c r="AF183" t="inlineStr"/>
       <c r="AG183" t="inlineStr"/>
+      <c r="AH183" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -17666,7 +18577,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H184" t="inlineStr"/>
@@ -17682,7 +18593,7 @@
       </c>
       <c r="O184" t="inlineStr">
         <is>
-          <t>Burndown, Team total available hours, Cycle time, Horas extras</t>
+          <t>Burndown, Team total available hours, Cycle time</t>
         </is>
       </c>
       <c r="P184" t="inlineStr">
@@ -17719,6 +18630,11 @@
       <c r="AE184" t="inlineStr"/>
       <c r="AF184" t="inlineStr"/>
       <c r="AG184" t="inlineStr"/>
+      <c r="AH184" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -17751,7 +18667,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Scrum, Lean</t>
+          <t>['Scrum', 'Lean']</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
@@ -17812,6 +18728,11 @@
       <c r="AE185" t="inlineStr"/>
       <c r="AF185" t="inlineStr"/>
       <c r="AG185" t="inlineStr"/>
+      <c r="AH185" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -17844,7 +18765,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Optamos por não adotar um framework e adequar o processo de acordo com a necessidade</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H186" t="inlineStr"/>
@@ -17909,6 +18830,11 @@
       <c r="AE186" t="inlineStr"/>
       <c r="AF186" t="inlineStr"/>
       <c r="AG186" t="inlineStr"/>
+      <c r="AH186" t="inlineStr">
+        <is>
+          <t>['Optamos por não adotar um framework e adequar o processo de acordo com a necessidade']</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -17941,7 +18867,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
@@ -18010,6 +18936,11 @@
       <c r="AE187" t="inlineStr"/>
       <c r="AF187" t="inlineStr"/>
       <c r="AG187" t="inlineStr"/>
+      <c r="AH187" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -18042,7 +18973,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Scrum, XP, Kanban, Lean</t>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
@@ -18107,6 +19038,11 @@
       <c r="AE188" t="inlineStr"/>
       <c r="AF188" t="inlineStr"/>
       <c r="AG188" t="inlineStr"/>
+      <c r="AH188" t="inlineStr">
+        <is>
+          <t>['Scrum', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -18139,7 +19075,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan</t>
+          <t>['Scrum', 'ScrumBan']</t>
         </is>
       </c>
       <c r="H189" t="inlineStr"/>
@@ -18196,6 +19132,11 @@
       <c r="AE189" t="inlineStr"/>
       <c r="AF189" t="inlineStr"/>
       <c r="AG189" t="inlineStr"/>
+      <c r="AH189" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -18228,7 +19169,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>ScrumBan, XP, Kanban, Lean</t>
+          <t>['ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
@@ -18289,6 +19230,11 @@
       <c r="AE190" t="inlineStr"/>
       <c r="AF190" t="inlineStr"/>
       <c r="AG190" t="inlineStr"/>
+      <c r="AH190" t="inlineStr">
+        <is>
+          <t>['ScrumBan', 'XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -18321,7 +19267,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban, Lean, Tradicional/PMI, etc.</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H191" t="inlineStr"/>
@@ -18394,6 +19340,11 @@
       <c r="AE191" t="inlineStr"/>
       <c r="AF191" t="inlineStr"/>
       <c r="AG191" t="inlineStr"/>
+      <c r="AH191" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban', 'Lean', 'Tradicional/PMI', 'etc.']</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -18426,7 +19377,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
@@ -18479,6 +19430,11 @@
       <c r="AE192" t="inlineStr"/>
       <c r="AF192" t="inlineStr"/>
       <c r="AG192" t="inlineStr"/>
+      <c r="AH192" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -18511,7 +19467,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -18572,6 +19528,11 @@
       <c r="AE193" t="inlineStr"/>
       <c r="AF193" t="inlineStr"/>
       <c r="AG193" t="inlineStr"/>
+      <c r="AH193" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -18604,7 +19565,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban']</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
@@ -18661,6 +19622,11 @@
       <c r="AE194" t="inlineStr"/>
       <c r="AF194" t="inlineStr"/>
       <c r="AG194" t="inlineStr"/>
+      <c r="AH194" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -18693,7 +19659,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H195" t="inlineStr"/>
@@ -18738,6 +19704,11 @@
       <c r="AE195" t="inlineStr"/>
       <c r="AF195" t="inlineStr"/>
       <c r="AG195" t="inlineStr"/>
+      <c r="AH195" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -18770,7 +19741,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -18827,6 +19798,11 @@
       <c r="AE196" t="inlineStr"/>
       <c r="AF196" t="inlineStr"/>
       <c r="AG196" t="inlineStr"/>
+      <c r="AH196" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -18859,7 +19835,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
@@ -18936,6 +19912,11 @@
       <c r="AE197" t="inlineStr"/>
       <c r="AF197" t="inlineStr"/>
       <c r="AG197" t="inlineStr"/>
+      <c r="AH197" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -18968,7 +19949,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
@@ -19021,6 +20002,11 @@
       <c r="AE198" t="inlineStr"/>
       <c r="AF198" t="inlineStr"/>
       <c r="AG198" t="inlineStr"/>
+      <c r="AH198" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -19053,7 +20039,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -19118,6 +20104,11 @@
       <c r="AE199" t="inlineStr"/>
       <c r="AF199" t="inlineStr"/>
       <c r="AG199" t="inlineStr"/>
+      <c r="AH199" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -19146,7 +20137,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, Kanban, Lean</t>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
@@ -19223,6 +20214,11 @@
       <c r="AE200" t="inlineStr"/>
       <c r="AF200" t="inlineStr"/>
       <c r="AG200" t="inlineStr"/>
+      <c r="AH200" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -19255,7 +20251,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan</t>
+          <t>['Scrum', 'ScrumBan']</t>
         </is>
       </c>
       <c r="H201" t="inlineStr"/>
@@ -19304,6 +20300,11 @@
       <c r="AE201" t="inlineStr"/>
       <c r="AF201" t="inlineStr"/>
       <c r="AG201" t="inlineStr"/>
+      <c r="AH201" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -19336,7 +20337,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Scrum, ScrumBan, XP, Kanban</t>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban']</t>
         </is>
       </c>
       <c r="H202" t="inlineStr"/>
@@ -19381,6 +20382,11 @@
       <c r="AE202" t="inlineStr"/>
       <c r="AF202" t="inlineStr"/>
       <c r="AG202" t="inlineStr"/>
+      <c r="AH202" t="inlineStr">
+        <is>
+          <t>['Scrum', 'ScrumBan', 'XP', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -19413,7 +20419,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
@@ -19462,6 +20468,11 @@
       <c r="AE203" t="inlineStr"/>
       <c r="AF203" t="inlineStr"/>
       <c r="AG203" t="inlineStr"/>
+      <c r="AH203" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -19494,7 +20505,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>XP, Kanban, Lean</t>
+          <t>['XP', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H204" t="inlineStr"/>
@@ -19543,6 +20554,11 @@
       <c r="AE204" t="inlineStr"/>
       <c r="AF204" t="inlineStr"/>
       <c r="AG204" t="inlineStr"/>
+      <c r="AH204" t="inlineStr">
+        <is>
+          <t>['XP', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -19575,7 +20591,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
@@ -19620,6 +20636,11 @@
       <c r="AE205" t="inlineStr"/>
       <c r="AF205" t="inlineStr"/>
       <c r="AG205" t="inlineStr"/>
+      <c r="AH205" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -19652,7 +20673,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Scrum, Kanban</t>
+          <t>['Scrum', 'Kanban']</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -19709,6 +20730,11 @@
       <c r="AE206" t="inlineStr"/>
       <c r="AF206" t="inlineStr"/>
       <c r="AG206" t="inlineStr"/>
+      <c r="AH206" t="inlineStr">
+        <is>
+          <t>['Scrum', 'Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -19741,7 +20767,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>ScrumBan, Kanban, Lean</t>
+          <t>['ScrumBan', 'Kanban', 'Lean']</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
@@ -19802,6 +20828,11 @@
       <c r="AE207" t="inlineStr"/>
       <c r="AF207" t="inlineStr"/>
       <c r="AG207" t="inlineStr"/>
+      <c r="AH207" t="inlineStr">
+        <is>
+          <t>['ScrumBan', 'Kanban', 'Lean']</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -19834,7 +20865,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Kanban</t>
+          <t>['Kanban']</t>
         </is>
       </c>
       <c r="H208" t="inlineStr"/>
@@ -19895,6 +20926,11 @@
       <c r="AE208" t="inlineStr"/>
       <c r="AF208" t="inlineStr"/>
       <c r="AG208" t="inlineStr"/>
+      <c r="AH208" t="inlineStr">
+        <is>
+          <t>['Kanban']</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -19927,7 +20963,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>ScrumBan</t>
+          <t>['ScrumBan']</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
@@ -19984,6 +21020,11 @@
       <c r="AE209" t="inlineStr"/>
       <c r="AF209" t="inlineStr"/>
       <c r="AG209" t="inlineStr"/>
+      <c r="AH209" t="inlineStr">
+        <is>
+          <t>['ScrumBan']</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -20016,7 +21057,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
@@ -20081,6 +21122,11 @@
       <c r="AE210" t="inlineStr"/>
       <c r="AF210" t="inlineStr"/>
       <c r="AG210" t="inlineStr"/>
+      <c r="AH210" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -20113,7 +21159,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Scrum</t>
+          <t>['Scrum']</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -20170,6 +21216,11 @@
       <c r="AE211" t="inlineStr"/>
       <c r="AF211" t="inlineStr"/>
       <c r="AG211" t="inlineStr"/>
+      <c r="AH211" t="inlineStr">
+        <is>
+          <t>['Scrum']</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>